<commit_message>
Verify bearing preload inlay depth.
</commit_message>
<xml_diff>
--- a/design_spreadsheets/Bearing Preload/Compliant Slider Preload.xlsx
+++ b/design_spreadsheets/Bearing Preload/Compliant Slider Preload.xlsx
@@ -86,7 +86,7 @@
     <t>actual preload force (N)</t>
   </si>
   <si>
-    <t>actual actual force penalty per patch (N)</t>
+    <t>actual actuation force penalty per patch (N)</t>
   </si>
 </sst>
 </file>
@@ -413,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,7 +463,7 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -472,7 +472,7 @@
       </c>
       <c r="B6">
         <f>B4*B5</f>
-        <v>1250</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -509,7 +509,7 @@
       </c>
       <c r="B11">
         <f>B10/B6</f>
-        <v>0.10666666666666667</v>
+        <v>5.3333333333333337E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -518,7 +518,7 @@
       </c>
       <c r="B12">
         <f>B11/B2</f>
-        <v>0.25847146900664197</v>
+        <v>0.12923573450332099</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -527,7 +527,7 @@
       </c>
       <c r="B13">
         <f>B12*B3</f>
-        <v>0.82064691409608825</v>
+        <v>0.41032345704804413</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -547,58 +547,62 @@
         <v>3.8249999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17">
         <f>B16-B13</f>
-        <v>3.0043530859039116</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3.4146765429519554</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
       <c r="B19">
         <f>ROUNDUP(B17,1)</f>
-        <v>3.1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
       <c r="B20">
         <f>(B16-B19)/B3</f>
-        <v>0.22834645669291329</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.10236220472440936</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
       <c r="B21">
         <f>B20*B2</f>
-        <v>9.4234599564068378E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4.2243096356306499E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
       <c r="B22">
         <f>B21*B6</f>
-        <v>117.79324945508547</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>105.60774089076625</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
       <c r="B23">
         <f>B22*B8</f>
-        <v>17.668987418262819</v>
+        <v>15.841161133614937</v>
+      </c>
+      <c r="J23">
+        <f>70.65+0.65*2+3.175</f>
+        <v>75.125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>